<commit_message>
Linked List Day-2 2qs Done
</commit_message>
<xml_diff>
--- a/DSA-Prep/DSA Sheet by Arsh (45 Days Plan).xlsx
+++ b/DSA-Prep/DSA Sheet by Arsh (45 Days Plan).xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="7990"/>
+    <workbookView windowWidth="19200" windowHeight="7750"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="882" uniqueCount="328">
   <si>
     <t>#CrackYourInternship Challenge</t>
   </si>
@@ -1024,10 +1024,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="36">
     <font>
@@ -1144,8 +1144,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1159,15 +1160,21 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1189,6 +1196,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -1202,13 +1216,6 @@
       <color theme="3"/>
       <name val="Arial"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1251,14 +1258,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Arial"/>
@@ -1268,7 +1267,15 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1276,13 +1283,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1323,37 +1323,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1371,7 +1395,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1383,25 +1419,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1413,19 +1431,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1437,13 +1455,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1461,49 +1497,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1517,13 +1517,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1591,39 +1604,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1635,130 +1635,130 @@
     <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2072,7 +2072,7 @@
   <dimension ref="A1:I340"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="B99" sqref="B99"/>
+      <selection activeCell="B102" sqref="B102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6272727272727" defaultRowHeight="15.75" customHeight="1"/>
@@ -3025,14 +3025,17 @@
       </c>
     </row>
     <row r="99" customHeight="1" spans="1:6">
-      <c r="A99" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B99" s="10" t="s">
+      <c r="A99" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B99" s="19" t="s">
         <v>101</v>
       </c>
+      <c r="C99" t="s">
+        <v>97</v>
+      </c>
       <c r="F99" s="5" t="s">
-        <v>9</v>
+        <v>98</v>
       </c>
     </row>
     <row r="100" customHeight="1" spans="1:6">
@@ -3047,14 +3050,17 @@
       </c>
     </row>
     <row r="101" customHeight="1" spans="1:6">
-      <c r="A101" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B101" s="10" t="s">
+      <c r="A101" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B101" s="19" t="s">
         <v>103</v>
       </c>
+      <c r="C101" t="s">
+        <v>97</v>
+      </c>
       <c r="F101" s="5" t="s">
-        <v>9</v>
+        <v>98</v>
       </c>
     </row>
     <row r="102" customHeight="1" spans="1:8">

</xml_diff>

<commit_message>
LL day - 3 done
</commit_message>
<xml_diff>
--- a/DSA-Prep/DSA Sheet by Arsh (45 Days Plan).xlsx
+++ b/DSA-Prep/DSA Sheet by Arsh (45 Days Plan).xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="7750"/>
+    <workbookView windowWidth="19200" windowHeight="7990"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="882" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="884" uniqueCount="328">
   <si>
     <t>#CrackYourInternship Challenge</t>
   </si>
@@ -1024,10 +1024,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="36">
     <font>
@@ -1144,11 +1144,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1160,23 +1167,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Arial"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1197,7 +1198,29 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1211,19 +1234,25 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Arial"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Arial"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1236,32 +1265,10 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="3"/>
       <name val="Arial"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Arial"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1282,14 +1289,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1323,7 +1323,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1335,7 +1353,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1347,7 +1365,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1359,103 +1425,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1473,25 +1449,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1503,7 +1485,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1517,26 +1517,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1556,11 +1556,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1589,21 +1595,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -1614,151 +1605,160 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="16" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="14" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="18" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="18" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -3081,14 +3081,17 @@
       </c>
     </row>
     <row r="103" customHeight="1" spans="1:4">
-      <c r="A103" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B103" s="10" t="s">
+      <c r="A103" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B103" s="19" t="s">
         <v>105</v>
       </c>
+      <c r="C103" t="s">
+        <v>97</v>
+      </c>
       <c r="D103" s="5" t="s">
-        <v>9</v>
+        <v>98</v>
       </c>
     </row>
     <row r="104" customHeight="1" spans="1:2">
@@ -3122,14 +3125,17 @@
       </c>
     </row>
     <row r="107" customHeight="1" spans="1:6">
-      <c r="A107" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B107" s="10" t="s">
+      <c r="A107" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B107" s="19" t="s">
         <v>109</v>
       </c>
+      <c r="C107" t="s">
+        <v>97</v>
+      </c>
       <c r="F107" s="5" t="s">
-        <v>9</v>
+        <v>98</v>
       </c>
     </row>
     <row r="108" customHeight="1" spans="1:7">

</xml_diff>

<commit_message>
Linked List Level - 1 done
</commit_message>
<xml_diff>
--- a/DSA-Prep/DSA Sheet by Arsh (45 Days Plan).xlsx
+++ b/DSA-Prep/DSA Sheet by Arsh (45 Days Plan).xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="894" uniqueCount="332">
   <si>
     <t>#CrackYourInternship Challenge</t>
   </si>
@@ -313,6 +313,9 @@
     <t>Yes</t>
   </si>
   <si>
+    <t>Imp</t>
+  </si>
+  <si>
     <t>https://leetcode.com/problems/linked-list-cycle/</t>
   </si>
   <si>
@@ -331,12 +334,18 @@
     <t>https://leetcode.com/problems/merge-two-sorted-lists/</t>
   </si>
   <si>
+    <t>V.Imp</t>
+  </si>
+  <si>
     <t>https://www.geeksforgeeks.org/multiply-two-numbers-represented-linked-lists/</t>
   </si>
   <si>
     <t>https://leetcode.com/problems/intersection-of-two-linked-lists/</t>
   </si>
   <si>
+    <t>Brute Force Done</t>
+  </si>
+  <si>
     <t>https://www.geeksforgeeks.org/given-only-a-pointer-to-a-node-to-be-deleted-in-a-singly-linked-list-how-do-you-delete-it/</t>
   </si>
   <si>
@@ -476,6 +485,9 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/range-sum-of-bst/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>https://leetcode.com/problems/symmetric-tree/</t>
@@ -1024,12 +1036,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="36">
+  <fonts count="37">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1121,6 +1133,14 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
@@ -1147,6 +1167,20 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -1158,11 +1192,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FF9C0006"/>
       <name val="Arial"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1174,24 +1207,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1236,8 +1269,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1252,7 +1301,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1260,36 +1309,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1323,7 +1343,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1335,37 +1385,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1377,61 +1421,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1455,13 +1457,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1473,13 +1487,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1491,19 +1505,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1514,6 +1534,47 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1541,21 +1602,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -1565,17 +1611,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1594,175 +1634,155 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="20" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="20" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="20" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="20" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="20" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="25" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="22" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
@@ -1805,10 +1825,11 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2074,8 +2095,8 @@
   </sheetPr>
   <dimension ref="A1:I340"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="B96" sqref="B96"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="C108" sqref="C108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6272727272727" defaultRowHeight="15.75" customHeight="1"/>
@@ -2979,7 +3000,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="96" customHeight="1" spans="1:7">
+    <row r="96" customHeight="1" spans="1:9">
       <c r="A96" s="17" t="s">
         <v>10</v>
       </c>
@@ -2995,13 +3016,16 @@
       <c r="G96" s="5" t="s">
         <v>98</v>
       </c>
+      <c r="I96" s="21" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="97" customHeight="1" spans="1:4">
       <c r="A97" s="17" t="s">
         <v>10</v>
       </c>
       <c r="B97" s="19" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C97" t="s">
         <v>97</v>
@@ -3010,12 +3034,12 @@
         <v>98</v>
       </c>
     </row>
-    <row r="98" customHeight="1" spans="1:6">
+    <row r="98" customHeight="1" spans="1:9">
       <c r="A98" s="17" t="s">
         <v>10</v>
       </c>
       <c r="B98" s="19" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C98" t="s">
         <v>97</v>
@@ -3026,13 +3050,16 @@
       <c r="F98" s="5" t="s">
         <v>98</v>
       </c>
+      <c r="I98" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="99" customHeight="1" spans="1:6">
       <c r="A99" s="17" t="s">
         <v>10</v>
       </c>
       <c r="B99" s="19" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C99" t="s">
         <v>97</v>
@@ -3046,7 +3073,7 @@
         <v>10</v>
       </c>
       <c r="B100" s="19" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C100" t="s">
         <v>97</v>
@@ -3060,7 +3087,7 @@
         <v>10</v>
       </c>
       <c r="B101" s="19" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C101" t="s">
         <v>97</v>
@@ -3069,21 +3096,27 @@
         <v>98</v>
       </c>
     </row>
-    <row r="102" customHeight="1" spans="1:8">
-      <c r="A102" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B102" s="10" t="s">
-        <v>104</v>
+    <row r="102" customHeight="1" spans="1:9">
+      <c r="A102" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B102" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="C102" t="s">
+        <v>97</v>
       </c>
       <c r="D102" s="5" t="s">
-        <v>9</v>
+        <v>98</v>
       </c>
       <c r="F102" s="5" t="s">
-        <v>9</v>
+        <v>98</v>
       </c>
       <c r="H102" s="5" t="s">
-        <v>9</v>
+        <v>98</v>
+      </c>
+      <c r="I102" s="21" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="103" customHeight="1" spans="1:4">
@@ -3091,7 +3124,7 @@
         <v>10</v>
       </c>
       <c r="B103" s="19" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C103" t="s">
         <v>97</v>
@@ -3100,12 +3133,15 @@
         <v>98</v>
       </c>
     </row>
-    <row r="104" customHeight="1" spans="1:2">
-      <c r="A104" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B104" s="10" t="s">
-        <v>106</v>
+    <row r="104" customHeight="1" spans="1:3">
+      <c r="A104" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B104" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="C104" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="105" customHeight="1" spans="1:6">
@@ -3113,7 +3149,7 @@
         <v>10</v>
       </c>
       <c r="B105" s="20" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="C105" t="s">
         <v>97</v>
@@ -3127,7 +3163,7 @@
         <v>10</v>
       </c>
       <c r="B106" s="19" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C106" t="s">
         <v>97</v>
@@ -3141,7 +3177,7 @@
         <v>10</v>
       </c>
       <c r="B107" s="19" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="C107" t="s">
         <v>97</v>
@@ -3151,14 +3187,17 @@
       </c>
     </row>
     <row r="108" customHeight="1" spans="1:7">
-      <c r="A108" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B108" s="10" t="s">
-        <v>110</v>
+      <c r="A108" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B108" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="C108" t="s">
+        <v>97</v>
       </c>
       <c r="G108" s="5" t="s">
-        <v>9</v>
+        <v>98</v>
       </c>
     </row>
     <row r="109" customHeight="1" spans="1:7">
@@ -3166,21 +3205,24 @@
         <v>20</v>
       </c>
       <c r="B109" s="10" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="G109" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="110" customHeight="1" spans="1:4">
-      <c r="A110" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B110" s="10" t="s">
-        <v>112</v>
+      <c r="A110" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B110" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="C110" t="s">
+        <v>97</v>
       </c>
       <c r="D110" s="5" t="s">
-        <v>9</v>
+        <v>98</v>
       </c>
     </row>
     <row r="111" customHeight="1" spans="1:2">
@@ -3188,7 +3230,7 @@
         <v>20</v>
       </c>
       <c r="B111" s="10" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="112" customHeight="1" spans="1:2">
@@ -3196,7 +3238,7 @@
         <v>20</v>
       </c>
       <c r="B112" s="10" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
     </row>
     <row r="113" customHeight="1" spans="1:8">
@@ -3204,7 +3246,7 @@
         <v>20</v>
       </c>
       <c r="B113" s="10" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="H113" s="5" t="s">
         <v>9</v>
@@ -3215,7 +3257,7 @@
         <v>20</v>
       </c>
       <c r="B114" s="10" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="H114" s="5" t="s">
         <v>9</v>
@@ -3226,7 +3268,7 @@
         <v>20</v>
       </c>
       <c r="B115" s="10" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="H115" s="5" t="s">
         <v>9</v>
@@ -3237,7 +3279,7 @@
         <v>20</v>
       </c>
       <c r="B116" s="10" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="F116" s="5" t="s">
         <v>9</v>
@@ -3248,7 +3290,7 @@
         <v>20</v>
       </c>
       <c r="B117" s="10" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="F117" s="5" t="s">
         <v>9</v>
@@ -3259,7 +3301,7 @@
         <v>20</v>
       </c>
       <c r="B118" s="10" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="F118" s="5" t="s">
         <v>9</v>
@@ -3270,7 +3312,7 @@
         <v>20</v>
       </c>
       <c r="B119" s="10" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
     </row>
     <row r="120" customHeight="1" spans="1:5">
@@ -3278,7 +3320,7 @@
         <v>20</v>
       </c>
       <c r="B120" s="10" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="E120" s="5" t="s">
         <v>9</v>
@@ -3289,7 +3331,7 @@
         <v>36</v>
       </c>
       <c r="B121" s="10" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
     </row>
     <row r="122" customHeight="1" spans="1:7">
@@ -3297,7 +3339,7 @@
         <v>36</v>
       </c>
       <c r="B122" s="10" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="G122" s="5" t="s">
         <v>9</v>
@@ -3308,7 +3350,7 @@
         <v>36</v>
       </c>
       <c r="B123" s="7" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="H123" s="5" t="s">
         <v>9</v>
@@ -3319,7 +3361,7 @@
         <v>36</v>
       </c>
       <c r="B124" s="7" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="H124" s="5" t="s">
         <v>9</v>
@@ -3330,7 +3372,7 @@
         <v>36</v>
       </c>
       <c r="B125" s="7" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="F125" s="5" t="s">
         <v>9</v>
@@ -3346,7 +3388,7 @@
     </row>
     <row r="127" customHeight="1" spans="2:4">
       <c r="B127" s="16" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D127" s="5" t="s">
         <v>9</v>
@@ -3360,7 +3402,7 @@
         <v>10</v>
       </c>
       <c r="B129" s="10" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="F129" s="5" t="s">
         <v>9</v>
@@ -3371,7 +3413,7 @@
         <v>10</v>
       </c>
       <c r="B130" s="10" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F130" s="5" t="s">
         <v>9</v>
@@ -3385,7 +3427,7 @@
         <v>10</v>
       </c>
       <c r="B131" s="10" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="H131" s="5" t="s">
         <v>9</v>
@@ -3395,8 +3437,8 @@
       <c r="A132" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B132" s="21" t="s">
-        <v>132</v>
+      <c r="B132" s="22" t="s">
+        <v>135</v>
       </c>
       <c r="F132" s="5" t="s">
         <v>9</v>
@@ -3410,7 +3452,7 @@
         <v>10</v>
       </c>
       <c r="B133" s="10" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="E133" s="5" t="s">
         <v>9</v>
@@ -3424,7 +3466,7 @@
         <v>10</v>
       </c>
       <c r="B134" s="10" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="E134" s="5" t="s">
         <v>9</v>
@@ -3437,8 +3479,8 @@
       <c r="A135" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B135" s="22" t="s">
-        <v>135</v>
+      <c r="B135" s="23" t="s">
+        <v>138</v>
       </c>
       <c r="E135" s="5" t="s">
         <v>9</v>
@@ -3449,7 +3491,7 @@
         <v>20</v>
       </c>
       <c r="B136" s="10" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="137" customHeight="1" spans="1:2">
@@ -3457,7 +3499,7 @@
         <v>20</v>
       </c>
       <c r="B137" s="10" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="138" customHeight="1" spans="1:2">
@@ -3465,7 +3507,7 @@
         <v>20</v>
       </c>
       <c r="B138" s="7" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
     </row>
     <row r="139" customHeight="1" spans="1:8">
@@ -3473,7 +3515,7 @@
         <v>20</v>
       </c>
       <c r="B139" s="10" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="H139" s="5" t="s">
         <v>9</v>
@@ -3484,7 +3526,7 @@
         <v>20</v>
       </c>
       <c r="B140" s="7" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="F140" s="5" t="s">
         <v>9</v>
@@ -3498,7 +3540,7 @@
         <v>20</v>
       </c>
       <c r="B141" s="10" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="F141" s="5" t="s">
         <v>9</v>
@@ -3512,7 +3554,7 @@
         <v>20</v>
       </c>
       <c r="B142" s="10" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="F142" s="5" t="s">
         <v>9</v>
@@ -3523,7 +3565,7 @@
         <v>20</v>
       </c>
       <c r="B143" s="7" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
     </row>
     <row r="144" customHeight="1" spans="1:2">
@@ -3531,7 +3573,7 @@
         <v>20</v>
       </c>
       <c r="B144" s="10" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
     </row>
     <row r="145" customHeight="1" spans="1:4">
@@ -3539,7 +3581,7 @@
         <v>20</v>
       </c>
       <c r="B145" s="10" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="D145" s="5" t="s">
         <v>9</v>
@@ -3550,7 +3592,7 @@
         <v>36</v>
       </c>
       <c r="B146" s="7" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D146" s="5" t="s">
         <v>9</v>
@@ -3561,7 +3603,7 @@
         <v>36</v>
       </c>
       <c r="B147" s="7" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="D147" s="5" t="s">
         <v>9</v>
@@ -3572,12 +3614,12 @@
         <v>36</v>
       </c>
       <c r="B148" s="7" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
     </row>
     <row r="151" customHeight="1" spans="2:2">
       <c r="B151" s="16" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
     </row>
     <row r="152" customHeight="1" spans="1:8">
@@ -3585,7 +3627,7 @@
         <v>10</v>
       </c>
       <c r="B152" s="10" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="H152" s="5" t="s">
         <v>9</v>
@@ -3596,7 +3638,7 @@
         <v>10</v>
       </c>
       <c r="B153" s="10" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="H153" s="5" t="s">
         <v>9</v>
@@ -3607,7 +3649,7 @@
         <v>10</v>
       </c>
       <c r="B154" s="10" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="H154" s="5" t="s">
         <v>9</v>
@@ -3618,15 +3660,15 @@
         <v>10</v>
       </c>
       <c r="B155" s="10" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
     </row>
     <row r="156" customHeight="1" spans="1:2">
       <c r="A156" s="5" t="s">
-        <v>10</v>
+        <v>157</v>
       </c>
       <c r="B156" s="10" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="157" customHeight="1" spans="1:4">
@@ -3634,7 +3676,7 @@
         <v>10</v>
       </c>
       <c r="B157" s="10" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="D157" s="5" t="s">
         <v>9</v>
@@ -3645,7 +3687,7 @@
         <v>10</v>
       </c>
       <c r="B158" s="10" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="D158" s="5" t="s">
         <v>9</v>
@@ -3656,7 +3698,7 @@
         <v>10</v>
       </c>
       <c r="B159" s="10" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="D159" s="5" t="s">
         <v>9</v>
@@ -3667,7 +3709,7 @@
         <v>10</v>
       </c>
       <c r="B160" s="10" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="F160" s="5" t="s">
         <v>9</v>
@@ -3678,7 +3720,7 @@
         <v>10</v>
       </c>
       <c r="B161" s="10" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="F161" s="5" t="s">
         <v>9</v>
@@ -3689,7 +3731,7 @@
         <v>10</v>
       </c>
       <c r="B162" s="10" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="F162" s="5" t="s">
         <v>9</v>
@@ -3700,7 +3742,7 @@
         <v>10</v>
       </c>
       <c r="B163" s="10" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
     </row>
     <row r="164" customHeight="1" spans="1:2">
@@ -3708,7 +3750,7 @@
         <v>10</v>
       </c>
       <c r="B164" s="10" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
     </row>
     <row r="165" customHeight="1" spans="1:2">
@@ -3716,7 +3758,7 @@
         <v>10</v>
       </c>
       <c r="B165" s="10" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
     </row>
     <row r="166" customHeight="1" spans="1:2">
@@ -3724,7 +3766,7 @@
         <v>10</v>
       </c>
       <c r="B166" s="10" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
     </row>
     <row r="167" customHeight="1" spans="1:2">
@@ -3732,7 +3774,7 @@
         <v>10</v>
       </c>
       <c r="B167" s="7" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
     </row>
     <row r="168" customHeight="1" spans="1:2">
@@ -3740,7 +3782,7 @@
         <v>10</v>
       </c>
       <c r="B168" s="10" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
     </row>
     <row r="169" customHeight="1" spans="1:2">
@@ -3748,7 +3790,7 @@
         <v>10</v>
       </c>
       <c r="B169" s="7" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
     </row>
     <row r="170" customHeight="1" spans="1:2">
@@ -3756,7 +3798,7 @@
         <v>20</v>
       </c>
       <c r="B170" s="10" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
     </row>
     <row r="171" customHeight="1" spans="1:4">
@@ -3764,7 +3806,7 @@
         <v>20</v>
       </c>
       <c r="B171" s="10" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="D171" s="5" t="s">
         <v>9</v>
@@ -3775,7 +3817,7 @@
         <v>20</v>
       </c>
       <c r="B172" s="10" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="D172" s="5" t="s">
         <v>9</v>
@@ -3786,7 +3828,7 @@
         <v>20</v>
       </c>
       <c r="B173" s="10" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D173" s="5" t="s">
         <v>9</v>
@@ -3797,7 +3839,7 @@
         <v>20</v>
       </c>
       <c r="B174" s="10" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
     </row>
     <row r="175" customHeight="1" spans="1:2">
@@ -3805,7 +3847,7 @@
         <v>20</v>
       </c>
       <c r="B175" s="10" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
     </row>
     <row r="176" customHeight="1" spans="1:2">
@@ -3813,7 +3855,7 @@
         <v>20</v>
       </c>
       <c r="B176" s="10" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
     </row>
     <row r="177" customHeight="1" spans="1:6">
@@ -3821,7 +3863,7 @@
         <v>20</v>
       </c>
       <c r="B177" s="10" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="F177" s="5" t="s">
         <v>9</v>
@@ -3832,7 +3874,7 @@
         <v>20</v>
       </c>
       <c r="B178" s="10" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="D178" s="5" t="s">
         <v>9</v>
@@ -3846,7 +3888,7 @@
         <v>20</v>
       </c>
       <c r="B179" s="10" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="D179" s="5" t="s">
         <v>9</v>
@@ -3860,7 +3902,7 @@
         <v>20</v>
       </c>
       <c r="B180" s="10" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="D180" s="5" t="s">
         <v>9</v>
@@ -3871,7 +3913,7 @@
         <v>20</v>
       </c>
       <c r="B181" s="10" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
     </row>
     <row r="182" customHeight="1" spans="1:2">
@@ -3879,7 +3921,7 @@
         <v>20</v>
       </c>
       <c r="B182" s="10" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
     </row>
     <row r="183" customHeight="1" spans="1:2">
@@ -3887,7 +3929,7 @@
         <v>20</v>
       </c>
       <c r="B183" s="10" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="184" customHeight="1" spans="1:6">
@@ -3895,7 +3937,7 @@
         <v>20</v>
       </c>
       <c r="B184" s="10" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="F184" s="5" t="s">
         <v>9</v>
@@ -3906,7 +3948,7 @@
         <v>20</v>
       </c>
       <c r="B185" s="10" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="F185" s="5" t="s">
         <v>9</v>
@@ -3917,7 +3959,7 @@
         <v>20</v>
       </c>
       <c r="B186" s="10" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="F186" s="5" t="s">
         <v>9</v>
@@ -3928,7 +3970,7 @@
         <v>20</v>
       </c>
       <c r="B187" s="10" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="E187" s="12" t="s">
         <v>9</v>
@@ -3939,15 +3981,15 @@
         <v>20</v>
       </c>
       <c r="B188" s="7" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
     </row>
     <row r="189" customHeight="1" spans="1:4">
       <c r="A189" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B189" s="22" t="s">
-        <v>187</v>
+      <c r="B189" s="23" t="s">
+        <v>191</v>
       </c>
       <c r="D189" s="5" t="s">
         <v>9</v>
@@ -3958,7 +4000,7 @@
         <v>36</v>
       </c>
       <c r="B190" s="10" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
     </row>
     <row r="191" customHeight="1" spans="1:2">
@@ -3966,7 +4008,7 @@
         <v>36</v>
       </c>
       <c r="B191" s="10" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
     </row>
     <row r="192" customHeight="1" spans="1:4">
@@ -3974,7 +4016,7 @@
         <v>36</v>
       </c>
       <c r="B192" s="10" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="D192" s="5" t="s">
         <v>9</v>
@@ -3985,7 +4027,7 @@
         <v>36</v>
       </c>
       <c r="B193" s="10" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="D193" s="5" t="s">
         <v>9</v>
@@ -3999,7 +4041,7 @@
         <v>36</v>
       </c>
       <c r="B194" s="10" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="D194" s="5" t="s">
         <v>9</v>
@@ -4016,7 +4058,7 @@
         <v>36</v>
       </c>
       <c r="B195" s="10" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
     </row>
     <row r="196" customHeight="1" spans="1:2">
@@ -4024,7 +4066,7 @@
         <v>36</v>
       </c>
       <c r="B196" s="10" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
     </row>
     <row r="197" customHeight="1" spans="1:6">
@@ -4032,7 +4074,7 @@
         <v>36</v>
       </c>
       <c r="B197" s="7" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="F197" s="5" t="s">
         <v>9</v>
@@ -4043,7 +4085,7 @@
         <v>36</v>
       </c>
       <c r="B198" s="7" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="F198" s="5" t="s">
         <v>9</v>
@@ -4054,12 +4096,12 @@
         <v>36</v>
       </c>
       <c r="B199" s="7" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
     </row>
     <row r="201" customHeight="1" spans="2:2">
       <c r="B201" s="5" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
     </row>
     <row r="202" customHeight="1" spans="1:2">
@@ -4067,7 +4109,7 @@
         <v>10</v>
       </c>
       <c r="B202" s="7" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
     </row>
     <row r="203" customHeight="1" spans="1:6">
@@ -4075,7 +4117,7 @@
         <v>10</v>
       </c>
       <c r="B203" s="7" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="F203" s="5" t="s">
         <v>9</v>
@@ -4086,7 +4128,7 @@
         <v>10</v>
       </c>
       <c r="B204" s="7" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="E204" s="5" t="s">
         <v>9</v>
@@ -4097,7 +4139,7 @@
         <v>10</v>
       </c>
       <c r="B205" s="7" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="E205" s="5" t="s">
         <v>9</v>
@@ -4108,7 +4150,7 @@
         <v>10</v>
       </c>
       <c r="B206" s="7" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="H206" s="5" t="s">
         <v>9</v>
@@ -4119,7 +4161,7 @@
         <v>10</v>
       </c>
       <c r="B207" s="7" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="F207" s="5" t="s">
         <v>9</v>
@@ -4130,7 +4172,7 @@
         <v>10</v>
       </c>
       <c r="B208" s="7" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="D208" s="5" t="s">
         <v>9</v>
@@ -4141,7 +4183,7 @@
         <v>20</v>
       </c>
       <c r="B209" s="7" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
     </row>
     <row r="210" customHeight="1" spans="1:8">
@@ -4149,7 +4191,7 @@
         <v>20</v>
       </c>
       <c r="B210" s="8" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="H210" s="5" t="s">
         <v>9</v>
@@ -4160,7 +4202,7 @@
         <v>20</v>
       </c>
       <c r="B211" s="8" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="E211" s="5" t="s">
         <v>9</v>
@@ -4174,7 +4216,7 @@
         <v>20</v>
       </c>
       <c r="B212" s="7" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="E212" s="5" t="s">
         <v>9</v>
@@ -4185,7 +4227,7 @@
         <v>20</v>
       </c>
       <c r="B213" s="7" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
     </row>
     <row r="214" customHeight="1" spans="1:6">
@@ -4193,7 +4235,7 @@
         <v>20</v>
       </c>
       <c r="B214" s="7" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="F214" s="5" t="s">
         <v>9</v>
@@ -4204,7 +4246,7 @@
         <v>20</v>
       </c>
       <c r="B215" s="7" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="D215" s="5" t="s">
         <v>9</v>
@@ -4215,7 +4257,7 @@
         <v>20</v>
       </c>
       <c r="B216" s="7" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
     </row>
     <row r="217" customHeight="1" spans="1:2">
@@ -4223,7 +4265,7 @@
         <v>20</v>
       </c>
       <c r="B217" s="7" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
     </row>
     <row r="218" customHeight="1" spans="1:2">
@@ -4231,7 +4273,7 @@
         <v>20</v>
       </c>
       <c r="B218" s="7" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
     </row>
     <row r="219" customHeight="1" spans="1:6">
@@ -4239,7 +4281,7 @@
         <v>20</v>
       </c>
       <c r="B219" s="7" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="F219" s="5" t="s">
         <v>9</v>
@@ -4250,7 +4292,7 @@
         <v>20</v>
       </c>
       <c r="B220" s="7" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="E220" s="5" t="s">
         <v>9</v>
@@ -4261,7 +4303,7 @@
         <v>20</v>
       </c>
       <c r="B221" s="7" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="D221" s="5" t="s">
         <v>9</v>
@@ -4275,7 +4317,7 @@
         <v>20</v>
       </c>
       <c r="B222" s="7" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="D222" s="5" t="s">
         <v>9</v>
@@ -4286,7 +4328,7 @@
         <v>20</v>
       </c>
       <c r="B223" s="7" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="F223" s="5" t="s">
         <v>9</v>
@@ -4297,7 +4339,7 @@
         <v>20</v>
       </c>
       <c r="B224" s="7" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="H224" s="5" t="s">
         <v>9</v>
@@ -4308,7 +4350,7 @@
         <v>20</v>
       </c>
       <c r="B225" s="7" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="E225" s="5" t="s">
         <v>9</v>
@@ -4319,7 +4361,7 @@
         <v>20</v>
       </c>
       <c r="B226" s="7" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="E226" s="5" t="s">
         <v>9</v>
@@ -4330,7 +4372,7 @@
         <v>20</v>
       </c>
       <c r="B227" s="7" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="F227" s="5" t="s">
         <v>9</v>
@@ -4341,7 +4383,7 @@
         <v>20</v>
       </c>
       <c r="B228" s="7" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="D228" s="5" t="s">
         <v>9</v>
@@ -4352,7 +4394,7 @@
         <v>36</v>
       </c>
       <c r="B229" s="8" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="D229" s="5" t="s">
         <v>9</v>
@@ -4363,7 +4405,7 @@
         <v>36</v>
       </c>
       <c r="B230" s="8" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="D230" s="5" t="s">
         <v>9</v>
@@ -4374,7 +4416,7 @@
         <v>36</v>
       </c>
       <c r="B231" s="8" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
     </row>
     <row r="232" customHeight="1" spans="1:2">
@@ -4382,7 +4424,7 @@
         <v>36</v>
       </c>
       <c r="B232" s="8" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
     </row>
     <row r="233" customHeight="1" spans="1:8">
@@ -4390,7 +4432,7 @@
         <v>36</v>
       </c>
       <c r="B233" s="7" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="H233" s="5" t="s">
         <v>9</v>
@@ -4401,7 +4443,7 @@
         <v>36</v>
       </c>
       <c r="B234" s="7" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="F234" s="5" t="s">
         <v>9</v>
@@ -4412,7 +4454,7 @@
         <v>36</v>
       </c>
       <c r="B235" s="7" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="E235" s="5" t="s">
         <v>9</v>
@@ -4423,7 +4465,7 @@
         <v>36</v>
       </c>
       <c r="B236" s="7" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="E236" s="5" t="s">
         <v>9</v>
@@ -4434,7 +4476,7 @@
         <v>36</v>
       </c>
       <c r="B237" s="7" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="F237" s="5" t="s">
         <v>9</v>
@@ -4445,7 +4487,7 @@
         <v>36</v>
       </c>
       <c r="B238" s="7" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
     </row>
     <row r="239" customHeight="1" spans="4:4">
@@ -4455,7 +4497,7 @@
     </row>
     <row r="240" customHeight="1" spans="2:2">
       <c r="B240" s="5" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
     </row>
     <row r="241" customHeight="1" spans="1:5">
@@ -4463,7 +4505,7 @@
         <v>20</v>
       </c>
       <c r="B241" s="7" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="E241" s="5" t="s">
         <v>9</v>
@@ -4474,7 +4516,7 @@
         <v>20</v>
       </c>
       <c r="B242" s="7" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="E242" s="5" t="s">
         <v>9</v>
@@ -4488,7 +4530,7 @@
         <v>20</v>
       </c>
       <c r="B243" s="7" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="F243" s="5" t="s">
         <v>9</v>
@@ -4499,7 +4541,7 @@
         <v>20</v>
       </c>
       <c r="B244" s="7" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
     </row>
     <row r="245" customHeight="1" spans="1:5">
@@ -4507,7 +4549,7 @@
         <v>36</v>
       </c>
       <c r="B245" s="7" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="E245" s="5" t="s">
         <v>9</v>
@@ -4518,7 +4560,7 @@
         <v>36</v>
       </c>
       <c r="B246" s="7" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="D246" s="5"/>
     </row>
@@ -4529,24 +4571,24 @@
       </c>
     </row>
     <row r="248" customHeight="1" spans="2:2">
-      <c r="B248" s="23" t="s">
-        <v>243</v>
+      <c r="B248" s="24" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="250" customHeight="1" spans="1:2">
       <c r="A250" s="5" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="B250" s="10" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
     </row>
     <row r="251" customHeight="1" spans="1:6">
       <c r="A251" s="5" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="B251" s="10" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="F251" s="5" t="s">
         <v>9</v>
@@ -4554,10 +4596,10 @@
     </row>
     <row r="252" customHeight="1" spans="1:6">
       <c r="A252" s="5" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="B252" s="10" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="F252" s="5" t="s">
         <v>9</v>
@@ -4565,10 +4607,10 @@
     </row>
     <row r="253" customHeight="1" spans="1:8">
       <c r="A253" s="5" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="B253" s="10" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="H253" s="5" t="s">
         <v>9</v>
@@ -4576,18 +4618,18 @@
     </row>
     <row r="254" customHeight="1" spans="1:2">
       <c r="A254" s="5" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="B254" s="10" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
     </row>
     <row r="255" customHeight="1" spans="1:6">
       <c r="A255" s="5" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="B255" s="10" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="E255" s="5" t="s">
         <v>9</v>
@@ -4598,18 +4640,18 @@
     </row>
     <row r="256" customHeight="1" spans="1:2">
       <c r="A256" s="5" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="B256" s="10" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
     </row>
     <row r="257" customHeight="1" spans="1:8">
       <c r="A257" s="5" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="B257" s="7" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="D257" s="5" t="s">
         <v>9</v>
@@ -4620,10 +4662,10 @@
     </row>
     <row r="258" customHeight="1" spans="1:6">
       <c r="A258" s="5" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="B258" s="7" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="D258" s="5" t="s">
         <v>9</v>
@@ -4634,10 +4676,10 @@
     </row>
     <row r="259" customHeight="1" spans="1:2">
       <c r="A259" s="5" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="B259" s="10" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
     </row>
     <row r="260" customHeight="1" spans="1:2">
@@ -4645,7 +4687,7 @@
         <v>36</v>
       </c>
       <c r="B260" s="8" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
     </row>
     <row r="261" customHeight="1" spans="1:5">
@@ -4653,7 +4695,7 @@
         <v>36</v>
       </c>
       <c r="B261" s="7" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="D261" s="5" t="s">
         <v>9</v>
@@ -4667,7 +4709,7 @@
         <v>36</v>
       </c>
       <c r="B262" s="7" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
     </row>
     <row r="263" customHeight="1" spans="1:8">
@@ -4675,7 +4717,7 @@
         <v>36</v>
       </c>
       <c r="B263" s="7" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="E263" s="5" t="s">
         <v>9</v>
@@ -4689,7 +4731,7 @@
     </row>
     <row r="265" customHeight="1" spans="2:2">
       <c r="B265" s="5" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
     </row>
     <row r="266" customHeight="1" spans="1:2">
@@ -4697,7 +4739,7 @@
         <v>10</v>
       </c>
       <c r="B266" s="7" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
     </row>
     <row r="267" customHeight="1" spans="1:2">
@@ -4705,7 +4747,7 @@
         <v>10</v>
       </c>
       <c r="B267" s="7" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
     </row>
     <row r="268" customHeight="1" spans="1:2">
@@ -4713,7 +4755,7 @@
         <v>10</v>
       </c>
       <c r="B268" s="7" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
     </row>
     <row r="269" customHeight="1" spans="1:6">
@@ -4721,7 +4763,7 @@
         <v>10</v>
       </c>
       <c r="B269" s="8" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="F269" s="5" t="s">
         <v>9</v>
@@ -4732,7 +4774,7 @@
         <v>20</v>
       </c>
       <c r="B270" s="10" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="D270" s="5" t="s">
         <v>9</v>
@@ -4746,7 +4788,7 @@
         <v>20</v>
       </c>
       <c r="B271" s="7" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="D271" s="5" t="s">
         <v>9</v>
@@ -4760,7 +4802,7 @@
         <v>20</v>
       </c>
       <c r="B272" s="10" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
     </row>
     <row r="273" customHeight="1" spans="1:2">
@@ -4768,7 +4810,7 @@
         <v>20</v>
       </c>
       <c r="B273" s="7" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
     </row>
     <row r="274" customHeight="1" spans="1:2">
@@ -4776,7 +4818,7 @@
         <v>20</v>
       </c>
       <c r="B274" s="7" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
     </row>
     <row r="275" customHeight="1" spans="1:6">
@@ -4784,7 +4826,7 @@
         <v>20</v>
       </c>
       <c r="B275" s="7" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="E275" s="5" t="s">
         <v>9</v>
@@ -4798,7 +4840,7 @@
         <v>20</v>
       </c>
       <c r="B276" s="7" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="E276" s="5" t="s">
         <v>9</v>
@@ -4812,7 +4854,7 @@
         <v>20</v>
       </c>
       <c r="B277" s="10" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="D277" s="5" t="s">
         <v>9</v>
@@ -4826,7 +4868,7 @@
         <v>20</v>
       </c>
       <c r="B278" s="7" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
     </row>
     <row r="279" customHeight="1" spans="1:2">
@@ -4834,7 +4876,7 @@
         <v>20</v>
       </c>
       <c r="B279" s="10" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
     </row>
     <row r="280" customHeight="1" spans="1:2">
@@ -4842,7 +4884,7 @@
         <v>20</v>
       </c>
       <c r="B280" s="7" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
     </row>
     <row r="281" customHeight="1" spans="1:6">
@@ -4850,7 +4892,7 @@
         <v>20</v>
       </c>
       <c r="B281" s="7" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="D281" s="5" t="s">
         <v>9</v>
@@ -4864,7 +4906,7 @@
         <v>20</v>
       </c>
       <c r="B282" s="7" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
     </row>
     <row r="283" customHeight="1" spans="1:2">
@@ -4872,7 +4914,7 @@
         <v>20</v>
       </c>
       <c r="B283" s="7" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
     </row>
     <row r="284" customHeight="1" spans="1:8">
@@ -4880,7 +4922,7 @@
         <v>20</v>
       </c>
       <c r="B284" s="10" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="E284" s="5" t="s">
         <v>9</v>
@@ -4894,7 +4936,7 @@
         <v>36</v>
       </c>
       <c r="B285" s="7" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="E285" s="5" t="s">
         <v>9</v>
@@ -4908,7 +4950,7 @@
         <v>36</v>
       </c>
       <c r="B286" s="10" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
     </row>
     <row r="287" customHeight="1" spans="1:4">
@@ -4916,7 +4958,7 @@
         <v>36</v>
       </c>
       <c r="B287" s="10" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="D287" s="5" t="s">
         <v>9</v>
@@ -4927,7 +4969,7 @@
         <v>36</v>
       </c>
       <c r="B288" s="10" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
     </row>
     <row r="289" customHeight="1" spans="1:6">
@@ -4935,7 +4977,7 @@
         <v>36</v>
       </c>
       <c r="B289" s="8" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="E289" s="5" t="s">
         <v>9</v>
@@ -4949,7 +4991,7 @@
         <v>36</v>
       </c>
       <c r="B290" s="7" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="E290" s="5" t="s">
         <v>9</v>
@@ -4960,7 +5002,7 @@
         <v>36</v>
       </c>
       <c r="B291" s="10" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="D291" s="5" t="s">
         <v>9</v>
@@ -4974,7 +5016,7 @@
         <v>36</v>
       </c>
       <c r="B292" s="10" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
     </row>
     <row r="293" customHeight="1" spans="1:8">
@@ -4982,7 +5024,7 @@
         <v>36</v>
       </c>
       <c r="B293" s="7" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="F293" s="5" t="s">
         <v>9</v>
@@ -4996,7 +5038,7 @@
         <v>36</v>
       </c>
       <c r="B294" s="10" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
     </row>
     <row r="295" customHeight="1" spans="1:5">
@@ -5004,7 +5046,7 @@
         <v>36</v>
       </c>
       <c r="B295" s="10" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="E295" s="5" t="s">
         <v>9</v>
@@ -5018,7 +5060,7 @@
     </row>
     <row r="297" customHeight="1" spans="2:2">
       <c r="B297" s="5" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
     </row>
     <row r="298" customHeight="1" spans="1:6">
@@ -5037,7 +5079,7 @@
         <v>20</v>
       </c>
       <c r="B299" s="10" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="D299" s="5" t="s">
         <v>9</v>
@@ -5048,7 +5090,7 @@
         <v>20</v>
       </c>
       <c r="B300" s="10" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="F300" s="5" t="s">
         <v>9</v>
@@ -5056,15 +5098,15 @@
     </row>
     <row r="303" customHeight="1" spans="2:2">
       <c r="B303" s="5" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
     </row>
     <row r="304" customHeight="1" spans="1:6">
       <c r="A304" s="5" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="B304" s="10" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="F304" s="5" t="s">
         <v>9</v>
@@ -5072,10 +5114,10 @@
     </row>
     <row r="305" customHeight="1" spans="1:7">
       <c r="A305" s="5" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="B305" s="10" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="D305" s="5" t="s">
         <v>9</v>
@@ -5086,26 +5128,26 @@
     </row>
     <row r="306" customHeight="1" spans="1:2">
       <c r="A306" s="5" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="B306" s="10" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
     </row>
     <row r="307" customHeight="1" spans="1:2">
       <c r="A307" s="5" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="B307" s="10" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
     </row>
     <row r="308" customHeight="1" spans="1:6">
       <c r="A308" s="5" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="B308" s="10" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="F308" s="5" t="s">
         <v>9</v>
@@ -5113,10 +5155,10 @@
     </row>
     <row r="309" customHeight="1" spans="1:4">
       <c r="A309" s="5" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="B309" s="10" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="D309" s="5" t="s">
         <v>9</v>
@@ -5124,10 +5166,10 @@
     </row>
     <row r="310" customHeight="1" spans="1:5">
       <c r="A310" s="5" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="B310" s="7" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="E310" s="5" t="s">
         <v>9</v>
@@ -5135,10 +5177,10 @@
     </row>
     <row r="311" customHeight="1" spans="1:8">
       <c r="A311" s="5" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="B311" s="10" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="H311" s="5" t="s">
         <v>9</v>
@@ -5146,10 +5188,10 @@
     </row>
     <row r="312" customHeight="1" spans="1:6">
       <c r="A312" s="5" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="B312" s="10" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="D312" s="5" t="s">
         <v>9</v>
@@ -5160,10 +5202,10 @@
     </row>
     <row r="313" customHeight="1" spans="1:8">
       <c r="A313" s="5" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="B313" s="7" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="D313" s="5" t="s">
         <v>9</v>
@@ -5177,7 +5219,7 @@
     </row>
     <row r="316" customHeight="1" spans="2:2">
       <c r="B316" s="16" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
     </row>
     <row r="317" customHeight="1" spans="1:2">
@@ -5185,7 +5227,7 @@
         <v>20</v>
       </c>
       <c r="B317" s="10" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
     </row>
     <row r="318" customHeight="1" spans="1:8">
@@ -5193,7 +5235,7 @@
         <v>20</v>
       </c>
       <c r="B318" s="8" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="F318" s="5" t="s">
         <v>9</v>
@@ -5207,7 +5249,7 @@
         <v>20</v>
       </c>
       <c r="B319" s="10" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="E319" s="5" t="s">
         <v>9</v>
@@ -5218,7 +5260,7 @@
         <v>20</v>
       </c>
       <c r="B320" s="10" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
     </row>
     <row r="321" customHeight="1" spans="1:7">
@@ -5226,7 +5268,7 @@
         <v>20</v>
       </c>
       <c r="B321" s="8" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="G321" s="5" t="s">
         <v>9</v>
@@ -5237,7 +5279,7 @@
         <v>20</v>
       </c>
       <c r="B322" s="10" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
     </row>
     <row r="323" customHeight="1" spans="1:5">
@@ -5245,7 +5287,7 @@
         <v>20</v>
       </c>
       <c r="B323" s="10" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="E323" s="5" t="s">
         <v>9</v>
@@ -5256,7 +5298,7 @@
         <v>20</v>
       </c>
       <c r="B324" s="10" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="H324" s="5" t="s">
         <v>9</v>
@@ -5267,7 +5309,7 @@
         <v>36</v>
       </c>
       <c r="B325" s="10" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
     </row>
     <row r="326" customHeight="1" spans="1:6">
@@ -5275,7 +5317,7 @@
         <v>36</v>
       </c>
       <c r="B326" s="10" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="E326" s="5" t="s">
         <v>9</v>
@@ -5289,7 +5331,7 @@
         <v>36</v>
       </c>
       <c r="B327" s="10" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="E327" s="5" t="s">
         <v>9</v>
@@ -5300,7 +5342,7 @@
         <v>36</v>
       </c>
       <c r="B328" s="10" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="D328" s="5" t="s">
         <v>9</v>
@@ -5314,7 +5356,7 @@
         <v>36</v>
       </c>
       <c r="B329" s="7" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
     </row>
     <row r="330" customHeight="1" spans="1:2">
@@ -5322,7 +5364,7 @@
         <v>36</v>
       </c>
       <c r="B330" s="7" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
     </row>
     <row r="331" customHeight="1" spans="1:7">
@@ -5330,7 +5372,7 @@
         <v>36</v>
       </c>
       <c r="B331" s="7" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="G331" s="5" t="s">
         <v>9</v>
@@ -5341,7 +5383,7 @@
         <v>36</v>
       </c>
       <c r="B332" s="7" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="D332" s="5" t="s">
         <v>9</v>
@@ -5355,7 +5397,7 @@
         <v>36</v>
       </c>
       <c r="B333" s="7" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
     </row>
     <row r="334" customHeight="1" spans="1:8">
@@ -5363,7 +5405,7 @@
         <v>36</v>
       </c>
       <c r="B334" s="7" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="H334" s="5" t="s">
         <v>9</v>
@@ -5375,8 +5417,8 @@
       </c>
     </row>
     <row r="336" customHeight="1" spans="2:5">
-      <c r="B336" s="24" t="s">
-        <v>323</v>
+      <c r="B336" s="25" t="s">
+        <v>327</v>
       </c>
       <c r="E336" s="5" t="s">
         <v>9</v>
@@ -5384,23 +5426,23 @@
     </row>
     <row r="337" customHeight="1" spans="1:2">
       <c r="A337" s="5" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="B337" s="7" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
     </row>
     <row r="338" customHeight="1" spans="1:2">
       <c r="A338" s="5" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="B338" s="7" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
     </row>
     <row r="339" customHeight="1" spans="1:8">
       <c r="A339" s="5" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="B339" s="7" t="s">
         <v>93</v>
@@ -5414,10 +5456,10 @@
     </row>
     <row r="340" customHeight="1" spans="1:2">
       <c r="A340" s="5" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="B340" s="7" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
     </row>
   </sheetData>

</xml_diff>